<commit_message>
replace NA and plot line graph
</commit_message>
<xml_diff>
--- a/dataset/dict_value.xlsx
+++ b/dataset/dict_value.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a72669bf9fc519c6/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a72669bf9fc519c6/Documents/Lab_Data Models [CPE213]/project213/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F087034-FC15-4260-BC22-ADD8C6B9EF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="8_{0F087034-FC15-4260-BC22-ADD8C6B9EF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88752AB0-4D63-4456-A70F-31546EF809FB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DEFD2951-C9BE-4F78-A2BC-2176574B7C21}"/>
+    <workbookView xWindow="2190" yWindow="2535" windowWidth="24645" windowHeight="13395" xr2:uid="{DEFD2951-C9BE-4F78-A2BC-2176574B7C21}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="284">
   <si>
     <t>Attribute</t>
   </si>
@@ -437,6 +437,456 @@
   </si>
   <si>
     <t>SNK</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>เพศ</t>
+  </si>
+  <si>
+    <t>ชาย</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>หญิง</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>job</t>
+  </si>
+  <si>
+    <t>งาน</t>
+  </si>
+  <si>
+    <t>นักท่องเที่ยว</t>
+  </si>
+  <si>
+    <t>tourist</t>
+  </si>
+  <si>
+    <t>พนักงานบริษัท/โรงงาน</t>
+  </si>
+  <si>
+    <t>employee</t>
+  </si>
+  <si>
+    <t>พนักงานขับรถโดยสาร/รถตู้/แท๊กซี่</t>
+  </si>
+  <si>
+    <t>driver</t>
+  </si>
+  <si>
+    <t>พ่อบ้าน/แม่บ้าน/ดูแลบ้าน</t>
+  </si>
+  <si>
+    <t>housekeeper</t>
+  </si>
+  <si>
+    <t>เด็กเล็ก/ในปกครอง</t>
+  </si>
+  <si>
+    <t>kid</t>
+  </si>
+  <si>
+    <t>มัคคุเทศก์/ไกด์ทัวร์</t>
+  </si>
+  <si>
+    <t>guide</t>
+  </si>
+  <si>
+    <t>ค้าขาย/ธุรกิจส่วนตัว</t>
+  </si>
+  <si>
+    <t>business</t>
+  </si>
+  <si>
+    <t>พยาบาล</t>
+  </si>
+  <si>
+    <t>nurse</t>
+  </si>
+  <si>
+    <t>ว่างงาน</t>
+  </si>
+  <si>
+    <t>unemployed</t>
+  </si>
+  <si>
+    <t>นักเรียน/นักศึกษา</t>
+  </si>
+  <si>
+    <t>student</t>
+  </si>
+  <si>
+    <t>ข้าราชการ/พนักงานของรัฐ / รัฐวิสาหกิจ</t>
+  </si>
+  <si>
+    <t>government</t>
+  </si>
+  <si>
+    <t>พนักงานในสถานบันเทิง</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entertainment </t>
+  </si>
+  <si>
+    <t>HCW (บุคลากรทางการแพทย์)</t>
+  </si>
+  <si>
+    <t>HCW</t>
+  </si>
+  <si>
+    <t>เจ้าหน้าที่สนามบิน</t>
+  </si>
+  <si>
+    <t>airport staff</t>
+  </si>
+  <si>
+    <t>รับจ้างทั่วไป / ฟรีแลนซ์</t>
+  </si>
+  <si>
+    <t>freelance</t>
+  </si>
+  <si>
+    <t>ไม่ระบุ</t>
+  </si>
+  <si>
+    <t>อื่นๆ</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>พนักงานร้านอาหาร</t>
+  </si>
+  <si>
+    <t>restaurant staff</t>
+  </si>
+  <si>
+    <t>เจ้าหน้าที่บนเครื่องบิน</t>
+  </si>
+  <si>
+    <t>cabin crew</t>
+  </si>
+  <si>
+    <t>เกษตรกร (ปลูกพืช)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farmer </t>
+  </si>
+  <si>
+    <t>พนักงานโรงแรม</t>
+  </si>
+  <si>
+    <t>hotel staff</t>
+  </si>
+  <si>
+    <t>แพทย์</t>
+  </si>
+  <si>
+    <t>doctor</t>
+  </si>
+  <si>
+    <t>risk</t>
+  </si>
+  <si>
+    <t>ความเสี่ยง</t>
+  </si>
+  <si>
+    <t>Cluster CBI โรงเบียร์ 90</t>
+  </si>
+  <si>
+    <t>Cluster Memory 90s กทม.</t>
+  </si>
+  <si>
+    <t>Cluster CBI beer</t>
+  </si>
+  <si>
+    <t>Cluster Memory 90s bkk</t>
+  </si>
+  <si>
+    <t>Cluster New Jazz กทม.</t>
+  </si>
+  <si>
+    <t>Cluster New Jazz bkk</t>
+  </si>
+  <si>
+    <t>Cluster ตลาดพรพัฒน์</t>
+  </si>
+  <si>
+    <t>Cluster pornpat market</t>
+  </si>
+  <si>
+    <t>Cluster บางแค</t>
+  </si>
+  <si>
+    <t>Cluster bangkae</t>
+  </si>
+  <si>
+    <t>ไปสถานที่แออัด เช่น งานแฟร์ คอนเสิร์ต</t>
+  </si>
+  <si>
+    <t>crowded place</t>
+  </si>
+  <si>
+    <t>ไปสถานที่ชุมชน เช่น ตลาดนัด สถานที่ท่องเที่ยว</t>
+  </si>
+  <si>
+    <t>community place</t>
+  </si>
+  <si>
+    <t>การค้นหาผู้ป่วยเชิงรุกและค้นหาผู้ติดเชื้อในชุมชน</t>
+  </si>
+  <si>
+    <t>proactive search</t>
+  </si>
+  <si>
+    <t>คนไทยเดินทางกลับจากต่างประเทศ</t>
+  </si>
+  <si>
+    <t>thai return</t>
+  </si>
+  <si>
+    <t>คนต่างชาติเดินทางมาจากต่างประเทศ</t>
+  </si>
+  <si>
+    <t>foreigners</t>
+  </si>
+  <si>
+    <t>ตรวจก่อนทำหัตถการ</t>
+  </si>
+  <si>
+    <t>medical procedure</t>
+  </si>
+  <si>
+    <t>บุคลากรด้านการแพทย์และสาธารณสุข</t>
+  </si>
+  <si>
+    <t>health personnel</t>
+  </si>
+  <si>
+    <t>ปอดอักเสบ (Pneumonia)</t>
+  </si>
+  <si>
+    <t>Pneumonia</t>
+  </si>
+  <si>
+    <t>ผู้ติดเชื้อในประเทศ</t>
+  </si>
+  <si>
+    <t>infected in country</t>
+  </si>
+  <si>
+    <t>ผู้ที่เดินทางมาจากต่างประเทศ และเข้า AOQ</t>
+  </si>
+  <si>
+    <t>AOQ</t>
+  </si>
+  <si>
+    <t>ผู้ที่เดินทางมาจากต่างประเทศ และเข้า ASQ/ALQ</t>
+  </si>
+  <si>
+    <t>ASQ/ALQ</t>
+  </si>
+  <si>
+    <t>ผู้ที่เดินทางมาจากต่างประเทศ และเข้า HQ/AHQ</t>
+  </si>
+  <si>
+    <t>HQ/AHQ</t>
+  </si>
+  <si>
+    <t>ผู้ที่เดินทางมาจากต่างประเทศ และเข้า OQ</t>
+  </si>
+  <si>
+    <t>OQ</t>
+  </si>
+  <si>
+    <t>พิธีกรรมทางศาสนา</t>
+  </si>
+  <si>
+    <t>religious ritual</t>
+  </si>
+  <si>
+    <t>ระบุไม่ได้</t>
+  </si>
+  <si>
+    <t>unspecified</t>
+  </si>
+  <si>
+    <t>ศูนย์กักกัน ผู้ต้องกัก</t>
+  </si>
+  <si>
+    <t>detention center</t>
+  </si>
+  <si>
+    <t>สถานบันเทิง</t>
+  </si>
+  <si>
+    <t>entertainment place</t>
+  </si>
+  <si>
+    <t>สนามมวย</t>
+  </si>
+  <si>
+    <t>boxing stadium</t>
+  </si>
+  <si>
+    <t>สัมผัสใกล้ชิดกับผู้ป่วยยืนยันรายก่อนหน้านี้</t>
+  </si>
+  <si>
+    <t>close contact</t>
+  </si>
+  <si>
+    <t>อยู่ระหว่างการสอบสวน</t>
+  </si>
+  <si>
+    <t>สัมผัสผู้เดินทางจากต่างประเทศ</t>
+  </si>
+  <si>
+    <t>อาชีพเสี่ยง เช่น ทำงานในสถานที่แออัด หรือทำงานใกล้ชิดสัมผัสชาวต่างชาติ เป็นต้น</t>
+  </si>
+  <si>
+    <t>under investigation</t>
+  </si>
+  <si>
+    <t>contact with travelers</t>
+  </si>
+  <si>
+    <t>risky career</t>
+  </si>
+  <si>
+    <t>patient_type_map</t>
+  </si>
+  <si>
+    <t>1.ผู้ป่วย PUI</t>
+  </si>
+  <si>
+    <t>PUI</t>
+  </si>
+  <si>
+    <t>10.อื่นๆ</t>
+  </si>
+  <si>
+    <t>2.สัมผัสผู้ติดเชื้อ</t>
+  </si>
+  <si>
+    <t>contact an infected person</t>
+  </si>
+  <si>
+    <t>3.ต่างชาติมาจากต่างประเทศ</t>
+  </si>
+  <si>
+    <t>4.คนไทยมาจากต่างประเทศ</t>
+  </si>
+  <si>
+    <t>5.ลักลอบเข้าประเทศ</t>
+  </si>
+  <si>
+    <t>smuggle</t>
+  </si>
+  <si>
+    <t>6.บุคลากรทางการแพทย์</t>
+  </si>
+  <si>
+    <t>7.เฝ้าระวัง ARI/pneumonia</t>
+  </si>
+  <si>
+    <t>ARI/pneumonia</t>
+  </si>
+  <si>
+    <t>8.สำรวจกลุ่มเสี่ยง (survey)</t>
+  </si>
+  <si>
+    <t>survey</t>
+  </si>
+  <si>
+    <t>9.ขอตรวจหาเชื้อเอง</t>
+  </si>
+  <si>
+    <t>self detect</t>
+  </si>
+  <si>
+    <t>ประมง/จับสัตว์น้ำ</t>
+  </si>
+  <si>
+    <t>Fishing</t>
+  </si>
+  <si>
+    <t>พยาบาลสูตินารีเวช</t>
+  </si>
+  <si>
+    <t>obstetrics nurse</t>
+  </si>
+  <si>
+    <t>พนักงานทำความสะอาด</t>
+  </si>
+  <si>
+    <t>cleaning staff</t>
+  </si>
+  <si>
+    <t>กรรมกร</t>
+  </si>
+  <si>
+    <t>labor</t>
+  </si>
+  <si>
+    <t>พนักงานนวด/สปา</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Massage </t>
+  </si>
+  <si>
+    <t>พระสงฆ์/สามเณร</t>
+  </si>
+  <si>
+    <t>monk</t>
+  </si>
+  <si>
+    <t>เกษตรกร (เลี้ยงสัตว์)</t>
+  </si>
+  <si>
+    <t>raising animals</t>
+  </si>
+  <si>
+    <t>พนักงานบริษัท</t>
+  </si>
+  <si>
+    <t>officer</t>
+  </si>
+  <si>
+    <t>อิสระ</t>
+  </si>
+  <si>
+    <t>independent staff</t>
+  </si>
+  <si>
+    <t>Cluster สมุทรสาคร</t>
+  </si>
+  <si>
+    <t>Cluster SKN</t>
+  </si>
+  <si>
+    <t>3.จากต่างประเทศ อยู่ใน Quarantine</t>
+  </si>
+  <si>
+    <t>Quarantine</t>
+  </si>
+  <si>
+    <t>8.ขอตรวจหาเชื้อเอง</t>
+  </si>
+  <si>
+    <t>7.สำรวจกลุ่มเสี่ยง (survey)</t>
+  </si>
+  <si>
+    <t>5.บุคลากรทางการแพทย์</t>
+  </si>
+  <si>
+    <t>6.เฝ้าระวัง ARI/ pneumonia</t>
   </si>
 </sst>
 </file>
@@ -799,17 +1249,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B351D090-DF76-41D6-A985-792670E170FC}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1"/>
-    <col min="3" max="4" width="17" customWidth="1"/>
+    <col min="3" max="3" width="73.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1336,12 +1787,657 @@
         <v>131</v>
       </c>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>132</v>
       </c>
       <c r="D65" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" t="s">
+        <v>135</v>
+      </c>
+      <c r="C67" t="s">
+        <v>136</v>
+      </c>
+      <c r="D67" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>138</v>
+      </c>
+      <c r="D68" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>140</v>
+      </c>
+      <c r="B69" t="s">
+        <v>141</v>
+      </c>
+      <c r="C69" t="s">
+        <v>142</v>
+      </c>
+      <c r="D69" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>144</v>
+      </c>
+      <c r="D70" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>146</v>
+      </c>
+      <c r="D71" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>148</v>
+      </c>
+      <c r="D72" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>150</v>
+      </c>
+      <c r="D73" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>152</v>
+      </c>
+      <c r="D74" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>154</v>
+      </c>
+      <c r="D75" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>156</v>
+      </c>
+      <c r="D76" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>158</v>
+      </c>
+      <c r="D77" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>160</v>
+      </c>
+      <c r="D78" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>162</v>
+      </c>
+      <c r="D79" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>164</v>
+      </c>
+      <c r="D80" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>166</v>
+      </c>
+      <c r="D81" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>168</v>
+      </c>
+      <c r="D82" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>170</v>
+      </c>
+      <c r="D83" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>172</v>
+      </c>
+      <c r="D84" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>173</v>
+      </c>
+      <c r="D85" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>175</v>
+      </c>
+      <c r="D86" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>177</v>
+      </c>
+      <c r="D87" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>179</v>
+      </c>
+      <c r="D88" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>181</v>
+      </c>
+      <c r="D89" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>266</v>
+      </c>
+      <c r="D90" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>268</v>
+      </c>
+      <c r="D91" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C92" t="s">
+        <v>272</v>
+      </c>
+      <c r="D92" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
+        <v>274</v>
+      </c>
+      <c r="D93" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>270</v>
+      </c>
+      <c r="D94" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
+        <v>264</v>
+      </c>
+      <c r="D95" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>262</v>
+      </c>
+      <c r="D96" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>260</v>
+      </c>
+      <c r="D97" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D98" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>183</v>
+      </c>
+      <c r="D99" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>185</v>
+      </c>
+      <c r="B100" t="s">
+        <v>186</v>
+      </c>
+      <c r="C100" t="s">
+        <v>187</v>
+      </c>
+      <c r="D100" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
+        <v>188</v>
+      </c>
+      <c r="D101" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
+        <v>191</v>
+      </c>
+      <c r="D102" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
+        <v>193</v>
+      </c>
+      <c r="D103" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C104" t="s">
+        <v>195</v>
+      </c>
+      <c r="D104" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
+        <v>197</v>
+      </c>
+      <c r="D105" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C106" t="s">
+        <v>199</v>
+      </c>
+      <c r="D106" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
+        <v>201</v>
+      </c>
+      <c r="D107" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
+        <v>203</v>
+      </c>
+      <c r="D108" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
+        <v>205</v>
+      </c>
+      <c r="D109" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C110" t="s">
+        <v>207</v>
+      </c>
+      <c r="D110" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
+        <v>209</v>
+      </c>
+      <c r="D111" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>211</v>
+      </c>
+      <c r="D112" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
+        <v>213</v>
+      </c>
+      <c r="D113" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
+        <v>215</v>
+      </c>
+      <c r="D114" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C115" t="s">
+        <v>217</v>
+      </c>
+      <c r="D115" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C116" t="s">
+        <v>219</v>
+      </c>
+      <c r="D116" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
+        <v>221</v>
+      </c>
+      <c r="D117" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>223</v>
+      </c>
+      <c r="D118" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C119" t="s">
+        <v>225</v>
+      </c>
+      <c r="D119" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C120" t="s">
+        <v>227</v>
+      </c>
+      <c r="D120" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C121" t="s">
+        <v>229</v>
+      </c>
+      <c r="D121" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
+        <v>231</v>
+      </c>
+      <c r="D122" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C123" t="s">
+        <v>233</v>
+      </c>
+      <c r="D123" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C124" t="s">
+        <v>235</v>
+      </c>
+      <c r="D124" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C125" t="s">
+        <v>236</v>
+      </c>
+      <c r="D125" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="126" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C126" t="s">
+        <v>237</v>
+      </c>
+      <c r="D126" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C127" t="s">
+        <v>276</v>
+      </c>
+      <c r="D127" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C129" t="s">
+        <v>173</v>
+      </c>
+      <c r="D129" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>241</v>
+      </c>
+      <c r="C130" t="s">
+        <v>242</v>
+      </c>
+      <c r="D130" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C131" t="s">
+        <v>244</v>
+      </c>
+      <c r="D131" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C132" t="s">
+        <v>245</v>
+      </c>
+      <c r="D132" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C133" t="s">
+        <v>247</v>
+      </c>
+      <c r="D133" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C134" t="s">
+        <v>248</v>
+      </c>
+      <c r="D134" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C135" t="s">
+        <v>249</v>
+      </c>
+      <c r="D135" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C136" t="s">
+        <v>251</v>
+      </c>
+      <c r="D136" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C137" t="s">
+        <v>252</v>
+      </c>
+      <c r="D137" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C138" t="s">
+        <v>254</v>
+      </c>
+      <c r="D138" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C139" t="s">
+        <v>256</v>
+      </c>
+      <c r="D139" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C141" t="s">
+        <v>278</v>
+      </c>
+      <c r="D141" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C142" t="s">
+        <v>280</v>
+      </c>
+      <c r="D142" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C143" t="s">
+        <v>281</v>
+      </c>
+      <c r="D143" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C144" t="s">
+        <v>282</v>
+      </c>
+      <c r="D144" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="145" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C145" t="s">
+        <v>283</v>
+      </c>
+      <c r="D145" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="146" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C146" t="s">
+        <v>280</v>
+      </c>
+      <c r="D146" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>